<commit_message>
2b1 z czterema wyjściami gotowe.
</commit_message>
<xml_diff>
--- a/02/sprawozdanie/Book1.xlsx
+++ b/02/sprawozdanie/Book1.xlsx
@@ -435,11 +435,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="527846208"/>
-        <c:axId val="527846784"/>
+        <c:axId val="526863168"/>
+        <c:axId val="526863744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="527846208"/>
+        <c:axId val="526863168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,12 +469,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527846784"/>
+        <c:crossAx val="526863744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="527846784"/>
+        <c:axId val="526863744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527846208"/>
+        <c:crossAx val="526863168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1842,11 +1842,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542609920"/>
-        <c:axId val="542610496"/>
+        <c:axId val="541495808"/>
+        <c:axId val="541496384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542609920"/>
+        <c:axId val="541495808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80000"/>
@@ -1878,12 +1878,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542610496"/>
+        <c:crossAx val="541496384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542610496"/>
+        <c:axId val="541496384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,7 +1915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542609920"/>
+        <c:crossAx val="541495808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3253,11 +3253,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542612800"/>
-        <c:axId val="542867456"/>
+        <c:axId val="541498688"/>
+        <c:axId val="541884416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542612800"/>
+        <c:axId val="541498688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80000"/>
@@ -3289,12 +3289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542867456"/>
+        <c:crossAx val="541884416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542867456"/>
+        <c:axId val="541884416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3326,7 +3326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542612800"/>
+        <c:crossAx val="541498688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4664,11 +4664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542869760"/>
-        <c:axId val="542870336"/>
+        <c:axId val="541886720"/>
+        <c:axId val="541887296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542869760"/>
+        <c:axId val="541886720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000"/>
@@ -4700,12 +4700,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542870336"/>
+        <c:crossAx val="541887296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542870336"/>
+        <c:axId val="541887296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4737,7 +4737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542869760"/>
+        <c:crossAx val="541886720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5084,11 +5084,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="527849088"/>
-        <c:axId val="527849664"/>
+        <c:axId val="526866048"/>
+        <c:axId val="526866624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="527849088"/>
+        <c:axId val="526866048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5118,12 +5118,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527849664"/>
+        <c:crossAx val="526866624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="527849664"/>
+        <c:axId val="526866624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5154,7 +5154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527849088"/>
+        <c:crossAx val="526866048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5505,11 +5505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541819456"/>
-        <c:axId val="541820032"/>
+        <c:axId val="541000256"/>
+        <c:axId val="541000832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541819456"/>
+        <c:axId val="541000256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5539,12 +5539,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541820032"/>
+        <c:crossAx val="541000832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541820032"/>
+        <c:axId val="541000832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5575,7 +5575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541819456"/>
+        <c:crossAx val="541000256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5940,11 +5940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541822336"/>
-        <c:axId val="541822912"/>
+        <c:axId val="541003136"/>
+        <c:axId val="541003712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541822336"/>
+        <c:axId val="541003136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5974,12 +5974,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541822912"/>
+        <c:crossAx val="541003712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541822912"/>
+        <c:axId val="541003712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6010,7 +6010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541822336"/>
+        <c:crossAx val="541003136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6382,11 +6382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541825216"/>
-        <c:axId val="541825792"/>
+        <c:axId val="541006016"/>
+        <c:axId val="541006592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541825216"/>
+        <c:axId val="541006016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6416,12 +6416,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541825792"/>
+        <c:crossAx val="541006592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541825792"/>
+        <c:axId val="541006592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6452,7 +6452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541825216"/>
+        <c:crossAx val="541006016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6824,11 +6824,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541942912"/>
-        <c:axId val="541943488"/>
+        <c:axId val="541090944"/>
+        <c:axId val="541091520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541942912"/>
+        <c:axId val="541090944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6858,12 +6858,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541943488"/>
+        <c:crossAx val="541091520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541943488"/>
+        <c:axId val="541091520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6894,7 +6894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541942912"/>
+        <c:crossAx val="541090944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6971,7 +6971,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7267,11 +7266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541945792"/>
-        <c:axId val="541946368"/>
+        <c:axId val="541093824"/>
+        <c:axId val="541094400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541945792"/>
+        <c:axId val="541093824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7295,19 +7294,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541946368"/>
+        <c:crossAx val="541094400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541946368"/>
+        <c:axId val="541094400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7332,21 +7330,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541945792"/>
+        <c:crossAx val="541093824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8677,11 +8673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="541948672"/>
-        <c:axId val="541949248"/>
+        <c:axId val="541096704"/>
+        <c:axId val="541097280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="541948672"/>
+        <c:axId val="541096704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000"/>
@@ -8713,12 +8709,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541949248"/>
+        <c:crossAx val="541097280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541949248"/>
+        <c:axId val="541097280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8750,7 +8746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541948672"/>
+        <c:crossAx val="541096704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10088,11 +10084,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542607040"/>
-        <c:axId val="542607616"/>
+        <c:axId val="541492928"/>
+        <c:axId val="541493504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542607040"/>
+        <c:axId val="541492928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000"/>
@@ -10124,12 +10120,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542607616"/>
+        <c:crossAx val="541493504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542607616"/>
+        <c:axId val="541493504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10161,7 +10157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542607040"/>
+        <c:crossAx val="541492928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14718,7 +14714,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>